<commit_message>
add Skill and Loop
</commit_message>
<xml_diff>
--- a/Assets/DataTable/XlsFile/DataTable_pre.xlsx
+++ b/Assets/DataTable/XlsFile/DataTable_pre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学校\授業使用\coly_project\Funkeln\Assets\DataTable\XlsFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Desktop/Project/Coly/Funkeln/Assets/DataTable/XlsFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812DBE4E-88F1-49B1-AD99-C6A4DD90850F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD6982-69A6-CB45-84DC-669B3C8676D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{1BBA983B-BC0B-4D31-AD3B-62B0C1995AF7}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="17280" windowHeight="8960" xr2:uid="{1BBA983B-BC0B-4D31-AD3B-62B0C1995AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Character" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -210,6 +210,9 @@
   <si>
     <t>SkillID4</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>SkillID1</t>
   </si>
 </sst>
 </file>
@@ -217,13 +220,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -242,7 +245,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -539,10 +542,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -553,7 +556,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -569,7 +572,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -867,19 +870,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463B50CB-D018-479A-8735-FB81A84DE7B7}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.19921875" customWidth="1"/>
-    <col min="7" max="7" width="11.69921875" customWidth="1"/>
-    <col min="8" max="8" width="13.796875" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,7 +929,7 @@
         <v>17</v>
       </c>
       <c r="P1" s="27" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="27" t="s">
         <v>44</v>
@@ -941,7 +944,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="16" thickBot="1">
       <c r="A2" s="4">
         <v>1000</v>
       </c>
@@ -988,22 +991,22 @@
         <v>5</v>
       </c>
       <c r="P2" s="28">
-        <v>1</v>
+        <v>9001000</v>
       </c>
       <c r="Q2" s="28">
-        <v>2</v>
+        <v>9001000</v>
       </c>
       <c r="R2" s="28">
-        <v>3</v>
+        <v>9001000</v>
       </c>
       <c r="S2" s="28">
-        <v>4</v>
+        <v>9001000</v>
       </c>
       <c r="T2" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8001000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="29" thickBot="1">
       <c r="A3" s="4">
         <v>2000</v>
       </c>
@@ -1049,8 +1052,23 @@
       <c r="O3" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="28">
+        <v>9002000</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>9002000</v>
+      </c>
+      <c r="R3" s="28">
+        <v>9002000</v>
+      </c>
+      <c r="S3" s="28">
+        <v>9002000</v>
+      </c>
+      <c r="T3" s="28">
+        <v>8001000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="16" thickBot="1">
       <c r="A4" s="4">
         <v>3000</v>
       </c>
@@ -1097,7 +1115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="16" thickBot="1">
       <c r="A5" s="4">
         <v>101000</v>
       </c>
@@ -1144,7 +1162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="16" thickBot="1">
       <c r="A6" s="4">
         <v>102000</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="16" thickBot="1">
       <c r="A7" s="4">
         <v>103000</v>
       </c>
@@ -1249,16 +1267,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999520B0-53BC-4391-B987-FDEDA7D46592}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1338,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="16" thickBot="1">
       <c r="A2" s="4">
         <v>4000</v>
       </c>
@@ -1367,7 +1385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="16" thickBot="1">
       <c r="A3" s="11">
         <v>104000</v>
       </c>
@@ -1429,17 +1447,17 @@
       <selection activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.796875" customWidth="1"/>
-    <col min="6" max="6" width="11.296875" customWidth="1"/>
-    <col min="7" max="7" width="12.796875" customWidth="1"/>
-    <col min="8" max="8" width="17.296875" customWidth="1"/>
-    <col min="9" max="9" width="12.796875" customWidth="1"/>
-    <col min="10" max="10" width="13.69921875" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1498,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="16" thickBot="1">
       <c r="A2" s="4">
         <v>1000</v>
       </c>
@@ -1510,7 +1528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="4">
         <v>2000</v>
       </c>
@@ -1540,7 +1558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="16" thickBot="1">
       <c r="A4" s="4">
         <v>3000</v>
       </c>
@@ -1584,16 +1602,16 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.296875" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="17.796875" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1634,7 +1652,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="16" thickBot="1">
       <c r="A2" s="4">
         <v>4000</v>
       </c>
@@ -1679,17 +1697,17 @@
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.296875" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" customWidth="1"/>
-    <col min="9" max="10" width="15.19921875" customWidth="1"/>
-    <col min="11" max="11" width="11.69921875" customWidth="1"/>
-    <col min="12" max="12" width="10.69921875" customWidth="1"/>
-    <col min="13" max="13" width="10.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="10" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="31" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1748,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="16" thickBot="1">
       <c r="B2" t="s">
         <v>27</v>
       </c>
@@ -1738,7 +1756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -1746,7 +1764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="16" thickBot="1">
       <c r="B4" t="s">
         <v>31</v>
       </c>
@@ -1768,20 +1786,20 @@
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="6" max="6" width="15.69921875" customWidth="1"/>
-    <col min="8" max="8" width="11.19921875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="11.19921875" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="15.796875" customWidth="1"/>
-    <col min="15" max="15" width="16.796875" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="16" thickBot="1">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -1841,7 +1859,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="B3" t="s">
         <v>37</v>
       </c>
@@ -1860,7 +1878,7 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13">
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -1872,7 +1890,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13">
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -1884,7 +1902,7 @@
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13">
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -1896,7 +1914,7 @@
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13">
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -1908,7 +1926,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13">
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
@@ -1920,7 +1938,7 @@
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13">
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -1932,7 +1950,7 @@
       <c r="K9" s="26"/>
       <c r="L9" s="26"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13">
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -1944,7 +1962,7 @@
       <c r="K10" s="26"/>
       <c r="L10" s="26"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13">
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -1956,7 +1974,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13">
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -1968,7 +1986,7 @@
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13">
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -1980,7 +1998,7 @@
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13">
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -1992,7 +2010,7 @@
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13">
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
@@ -2004,7 +2022,7 @@
       <c r="K15" s="26"/>
       <c r="L15" s="26"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13">
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
@@ -2016,7 +2034,7 @@
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:12">
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
@@ -2028,7 +2046,7 @@
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:12">
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
@@ -2040,7 +2058,7 @@
       <c r="K18" s="26"/>
       <c r="L18" s="26"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:12">
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
@@ -2052,7 +2070,7 @@
       <c r="K19" s="26"/>
       <c r="L19" s="26"/>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:12">
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
@@ -2064,7 +2082,7 @@
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:12">
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
@@ -2076,7 +2094,7 @@
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:12">
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
@@ -2088,7 +2106,7 @@
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:12">
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
@@ -2100,7 +2118,7 @@
       <c r="K23" s="26"/>
       <c r="L23" s="26"/>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:12">
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
@@ -2112,7 +2130,7 @@
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:12">
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
@@ -2124,7 +2142,7 @@
       <c r="K25" s="26"/>
       <c r="L25" s="26"/>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:12">
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="26"/>
@@ -2136,7 +2154,7 @@
       <c r="K26" s="26"/>
       <c r="L26" s="26"/>
     </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:12">
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
@@ -2148,7 +2166,7 @@
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:12">
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
@@ -2160,7 +2178,7 @@
       <c r="K28" s="26"/>
       <c r="L28" s="26"/>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:12">
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
@@ -2172,7 +2190,7 @@
       <c r="K29" s="26"/>
       <c r="L29" s="26"/>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:12">
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
       <c r="E30" s="26"/>
@@ -2184,7 +2202,7 @@
       <c r="K30" s="26"/>
       <c r="L30" s="26"/>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:12">
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
       <c r="E31" s="26"/>

</xml_diff>

<commit_message>
skill system and 102000 character
</commit_message>
<xml_diff>
--- a/Assets/DataTable/XlsFile/DataTable_pre.xlsx
+++ b/Assets/DataTable/XlsFile/DataTable_pre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Desktop/Project/Coly/Funkeln/Assets/DataTable/XlsFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD6982-69A6-CB45-84DC-669B3C8676D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4F65DB-13F0-DE4C-9F02-4AC24C3B4859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="17280" windowHeight="8960" xr2:uid="{1BBA983B-BC0B-4D31-AD3B-62B0C1995AF7}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>SkillID1</t>
+  </si>
+  <si>
+    <t>サファイア</t>
   </si>
 </sst>
 </file>
@@ -870,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463B50CB-D018-479A-8735-FB81A84DE7B7}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -887,61 +887,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="I1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="27" t="s">
         <v>41</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="16" thickBot="1">
@@ -1167,13 +1167,13 @@
         <v>102000</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C6" s="6">
         <v>10000</v>
       </c>
       <c r="D6" s="6">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="E6" s="6">
         <v>1000</v>
@@ -1185,7 +1185,7 @@
         <v>100</v>
       </c>
       <c r="H6" s="6">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="I6" s="6">
         <v>1000</v>
@@ -1207,6 +1207,21 @@
       </c>
       <c r="O6" s="7">
         <v>5</v>
+      </c>
+      <c r="P6" s="28">
+        <v>9001000</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>9001000</v>
+      </c>
+      <c r="R6" s="28">
+        <v>9001000</v>
+      </c>
+      <c r="S6" s="28">
+        <v>9102000</v>
+      </c>
+      <c r="T6" s="28">
+        <v>8102000</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="16" thickBot="1">
@@ -1214,7 +1229,7 @@
         <v>103000</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
         <v>10000</v>
@@ -1281,61 +1296,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="I1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="27" t="s">
         <v>41</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="27" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="16" thickBot="1">
@@ -1343,7 +1358,7 @@
         <v>4000</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="6">
         <v>3000</v>
@@ -1390,7 +1405,7 @@
         <v>104000</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="13">
         <v>50000</v>
@@ -1462,40 +1477,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1">
@@ -1504,10 +1519,10 @@
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="19">
         <v>25</v>
@@ -1519,13 +1534,13 @@
         <v>10</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
@@ -1534,10 +1549,10 @@
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="19">
         <v>25</v>
@@ -1549,13 +1564,13 @@
         <v>10</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16" thickBot="1">
@@ -1564,13 +1579,13 @@
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="18">
         <v>20</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="19">
         <v>25</v>
@@ -1616,40 +1631,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1">
@@ -1658,10 +1673,10 @@
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="19">
         <v>25</v>
@@ -1670,7 +1685,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="19">
         <v>50</v>
@@ -1712,64 +1727,64 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16" thickBot="1">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1804,45 +1819,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1">
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="25">
         <v>50</v>
@@ -1861,7 +1876,7 @@
     </row>
     <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25">

</xml_diff>

<commit_message>
hp bar & factory
</commit_message>
<xml_diff>
--- a/Assets/DataTable/XlsFile/DataTable_pre.xlsx
+++ b/Assets/DataTable/XlsFile/DataTable_pre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kk/Desktop/Project/Coly/Funkeln/Assets/DataTable/XlsFile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BC7945-7ABC-074E-A432-A6BB7944539D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6683993F-D921-4F4D-979F-9E5252481264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="17280" windowHeight="8960" activeTab="1" xr2:uid="{1BBA983B-BC0B-4D31-AD3B-62B0C1995AF7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>エメ</t>
+  </si>
+  <si>
+    <t>BossFlag</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999520B0-53BC-4391-B987-FDEDA7D46592}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1324,7 +1327,7 @@
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="29" thickBot="1">
+    <row r="1" spans="1:21" ht="29" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,8 +1388,11 @@
       <c r="T1" s="27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="29" thickBot="1">
+      <c r="U1" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="29" thickBot="1">
       <c r="A2" s="4">
         <v>4000</v>
       </c>
@@ -1447,8 +1453,11 @@
       <c r="T2" s="28">
         <v>8001000</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="29" thickBot="1">
+      <c r="U2" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="29" thickBot="1">
       <c r="A3" s="4">
         <v>5000</v>
       </c>
@@ -1509,8 +1518,11 @@
       <c r="T3" s="28">
         <v>8001000</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="16" thickBot="1">
+      <c r="U3" s="28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16" thickBot="1">
       <c r="A4" s="11">
         <v>104000</v>
       </c>
@@ -1570,6 +1582,9 @@
       </c>
       <c r="T4" s="28">
         <v>8104000</v>
+      </c>
+      <c r="U4" s="28" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>